<commit_message>
Updated defaults documents per Steve's questions
</commit_message>
<xml_diff>
--- a/GRAUML/Documentation/Annotation Defaults.xlsx
+++ b/GRAUML/Documentation/Annotation Defaults.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="449">
   <si>
     <t>Class</t>
   </si>
@@ -1705,9 +1705,6 @@
     <t>[today]</t>
   </si>
   <si>
-    <t>PIM - Actors in collaboration</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -1735,37 +1732,49 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Does "N" mean "false"?</t>
-  </si>
-  <si>
-    <t>Does "Y" mean "true"?</t>
-  </si>
-  <si>
     <t>PIM - ports on service component</t>
   </si>
   <si>
     <t>PIM: Use case</t>
   </si>
   <si>
-    <t>Says not derived, but provides default value. Which phase?</t>
-  </si>
-  <si>
     <t>Needs more detail</t>
   </si>
   <si>
-    <t>Actors in Package realized by Participant - also see Tom's email</t>
-  </si>
-  <si>
-    <t>"N/A" means literally insert "N/A", right?</t>
-  </si>
-  <si>
     <t>Boilerplate.</t>
+  </si>
+  <si>
+    <t>Does "N" mean "false"? [cbc] Yes</t>
+  </si>
+  <si>
+    <t>Does "Y" mean "true"? [cbc] Yes</t>
+  </si>
+  <si>
+    <t>"N/A" means literally insert "N/A", right? [cbc] Yes</t>
+  </si>
+  <si>
+    <t>PIM - Actors defined in service interactions or where an actor or package acontaining actors is explicitly realized by an ExchangePartner annotation instance.</t>
+  </si>
+  <si>
+    <t>PIM: Use case provider or consumer</t>
+  </si>
+  <si>
+    <t>Says not derived, but provides default value. Which phase? [cbc] done</t>
+  </si>
+  <si>
+    <t>Actors in Package realized by Participant - also see Tom's email  [cbc] done</t>
+  </si>
+  <si>
+    <t>[cbc] These defaults are a guess, there does not seem to be a default at the SDD level. Perhaps make them the same as WS RS SIP?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1811,7 +1820,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1827,13 +1836,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1894,7 +1899,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1929,7 +1934,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2140,8 +2145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,7 +2155,7 @@
     <col min="2" max="2" width="40" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="64.5703125" style="2" customWidth="1"/>
     <col min="7" max="16384" width="21.5703125" style="2"/>
   </cols>
@@ -2166,13 +2171,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2188,7 +2193,7 @@
       <c r="D2" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2203,11 +2208,11 @@
       <c r="D3" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>409</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2223,7 +2228,7 @@
       <c r="D4" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -2238,7 +2243,7 @@
       <c r="D5" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -2253,8 +2258,8 @@
       <c r="D6" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>430</v>
+      <c r="E6" s="4" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2270,7 +2275,7 @@
       <c r="D7" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -2285,9 +2290,9 @@
       <c r="D8" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -2300,8 +2305,11 @@
       <c r="D9" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>409</v>
+      <c r="E9" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2317,7 +2325,7 @@
       <c r="D10" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2334,7 +2342,7 @@
       <c r="D11" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2351,11 +2359,11 @@
       <c r="D12" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>408</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2371,7 +2379,7 @@
       <c r="D13" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2388,7 +2396,7 @@
       <c r="D14" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2405,7 +2413,7 @@
       <c r="D15" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2422,7 +2430,7 @@
       <c r="D16" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2439,7 +2447,7 @@
       <c r="D17" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2456,7 +2464,7 @@
       <c r="D18" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2473,7 +2481,7 @@
       <c r="D19" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2490,7 +2498,7 @@
       <c r="D20" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>408</v>
       </c>
     </row>
@@ -2507,7 +2515,7 @@
       <c r="D21" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2524,7 +2532,7 @@
       <c r="D22" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2541,7 +2549,7 @@
       <c r="D23" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -2556,8 +2564,8 @@
       <c r="D24" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>433</v>
+      <c r="E24" s="4" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2573,7 +2581,7 @@
       <c r="D25" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -2588,7 +2596,7 @@
       <c r="D26" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -2603,7 +2611,7 @@
       <c r="D27" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -2618,8 +2626,8 @@
       <c r="D28" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>434</v>
+      <c r="E28" s="4" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2635,7 +2643,7 @@
       <c r="D29" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="4" t="s">
         <v>424</v>
       </c>
     </row>
@@ -2652,7 +2660,7 @@
       <c r="D30" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -2667,7 +2675,7 @@
       <c r="D31" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
@@ -2682,7 +2690,7 @@
       <c r="D32" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E32" s="6"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -2697,7 +2705,7 @@
       <c r="D33" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
@@ -2712,7 +2720,7 @@
       <c r="D34" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
@@ -2727,7 +2735,7 @@
       <c r="D35" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
@@ -2742,8 +2750,8 @@
       <c r="D36" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>431</v>
+      <c r="E36" s="4" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2759,7 +2767,7 @@
       <c r="D37" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E37" s="6"/>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
@@ -2774,7 +2782,7 @@
       <c r="D38" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
@@ -2789,7 +2797,7 @@
       <c r="D39" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
@@ -2804,7 +2812,7 @@
       <c r="D40" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E40" s="6"/>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
@@ -2819,8 +2827,8 @@
       <c r="D41" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>432</v>
+      <c r="E41" s="4" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2836,7 +2844,7 @@
       <c r="D42" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="4" t="s">
         <v>425</v>
       </c>
     </row>
@@ -2853,7 +2861,7 @@
       <c r="D43" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
@@ -2868,7 +2876,7 @@
       <c r="D44" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E44" s="6"/>
+      <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
@@ -2883,7 +2891,7 @@
       <c r="D45" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E45" s="6"/>
+      <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
@@ -2898,7 +2906,7 @@
       <c r="D46" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E46" s="6"/>
+      <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
@@ -2913,7 +2921,7 @@
       <c r="D47" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
@@ -2928,7 +2936,7 @@
       <c r="D48" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E48" s="6"/>
+      <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
@@ -2943,7 +2951,7 @@
       <c r="D49" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E49" s="6"/>
+      <c r="E49" s="4"/>
     </row>
     <row r="50" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -2958,7 +2966,7 @@
       <c r="D50" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E50" s="6"/>
+      <c r="E50" s="4"/>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -2973,7 +2981,7 @@
       <c r="D51" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E51" s="6"/>
+      <c r="E51" s="4"/>
     </row>
     <row r="52" spans="1:6" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -2988,8 +2996,8 @@
       <c r="D52" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E52" s="6" t="s">
-        <v>440</v>
+      <c r="E52" s="4" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3005,7 +3013,7 @@
       <c r="D53" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E53" s="6"/>
+      <c r="E53" s="4"/>
     </row>
     <row r="54" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -3020,7 +3028,7 @@
       <c r="D54" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="E54" s="4" t="s">
         <v>426</v>
       </c>
     </row>
@@ -3037,7 +3045,7 @@
       <c r="D55" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E55" s="6"/>
+      <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:6" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
@@ -3052,7 +3060,7 @@
       <c r="D56" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E56" s="6"/>
+      <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
@@ -3067,11 +3075,11 @@
       <c r="D57" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="4" t="s">
         <v>414</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3087,7 +3095,7 @@
       <c r="D58" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E58" s="6"/>
+      <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:6" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
@@ -3102,7 +3110,7 @@
       <c r="D59" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E59" s="6"/>
+      <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
@@ -3117,7 +3125,7 @@
       <c r="D60" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="4" t="s">
         <v>427</v>
       </c>
     </row>
@@ -3134,7 +3142,7 @@
       <c r="D61" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="E61" s="4" t="s">
         <v>414</v>
       </c>
     </row>
@@ -3151,7 +3159,7 @@
       <c r="D62" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="E62" s="4" t="s">
         <v>414</v>
       </c>
     </row>
@@ -3168,9 +3176,9 @@
       <c r="D63" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="1:6" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>212</v>
       </c>
@@ -3183,11 +3191,11 @@
       <c r="D64" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="E64" s="6" t="s">
-        <v>428</v>
+      <c r="E64" s="4" t="s">
+        <v>444</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3203,11 +3211,11 @@
       <c r="D65" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E65" s="4" t="s">
         <v>423</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3223,7 +3231,7 @@
       <c r="D66" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E66" s="6"/>
+      <c r="E66" s="4"/>
     </row>
     <row r="67" spans="1:6" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
@@ -3238,7 +3246,7 @@
       <c r="D67" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="E67" s="4" t="s">
         <v>427</v>
       </c>
     </row>
@@ -3255,7 +3263,7 @@
       <c r="D68" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E68" s="6" t="s">
+      <c r="E68" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -3272,7 +3280,7 @@
       <c r="D69" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E69" s="6"/>
+      <c r="E69" s="4"/>
     </row>
     <row r="70" spans="1:6" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
@@ -3287,7 +3295,7 @@
       <c r="D70" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E70" s="6"/>
+      <c r="E70" s="4"/>
     </row>
     <row r="71" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
@@ -3302,7 +3310,7 @@
       <c r="D71" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E71" s="6"/>
+      <c r="E71" s="4"/>
     </row>
     <row r="72" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
@@ -3317,7 +3325,7 @@
       <c r="D72" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="E72" s="4" t="s">
         <v>414</v>
       </c>
     </row>
@@ -3334,7 +3342,7 @@
       <c r="D73" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E73" s="6" t="s">
+      <c r="E73" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -3351,8 +3359,8 @@
       <c r="D74" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="E74" s="6" t="s">
-        <v>441</v>
+      <c r="E74" s="4" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3368,7 +3376,7 @@
       <c r="D75" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E75" s="6"/>
+      <c r="E75" s="4"/>
     </row>
     <row r="76" spans="1:6" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
@@ -3381,13 +3389,13 @@
         <v>241</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E76" s="6">
+        <v>413</v>
+      </c>
+      <c r="E76" s="5">
         <v>1</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3403,7 +3411,7 @@
       <c r="D77" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E77" s="6" t="s">
+      <c r="E77" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -3420,7 +3428,7 @@
       <c r="D78" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E78" s="6" t="s">
+      <c r="E78" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -3437,7 +3445,7 @@
       <c r="D79" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E79" s="6"/>
+      <c r="E79" s="4"/>
     </row>
     <row r="80" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
@@ -3452,7 +3460,7 @@
       <c r="D80" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="E80" s="4" t="s">
         <v>414</v>
       </c>
     </row>
@@ -3469,7 +3477,7 @@
       <c r="D81" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E81" s="6"/>
+      <c r="E81" s="4"/>
     </row>
     <row r="82" spans="1:6" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
@@ -3484,7 +3492,7 @@
       <c r="D82" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E82" s="6"/>
+      <c r="E82" s="4"/>
     </row>
     <row r="83" spans="1:6" s="3" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
@@ -3500,7 +3508,7 @@
         <v>413</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3516,7 +3524,7 @@
       <c r="D84" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E84" s="6"/>
+      <c r="E84" s="4"/>
     </row>
     <row r="85" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
@@ -3531,8 +3539,8 @@
       <c r="D85" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E85" s="6" t="s">
-        <v>429</v>
+      <c r="E85" s="4" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3548,7 +3556,7 @@
       <c r="D86" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E86" s="6"/>
+      <c r="E86" s="4"/>
     </row>
     <row r="87" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
@@ -3563,7 +3571,7 @@
       <c r="D87" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E87" s="6"/>
+      <c r="E87" s="4"/>
     </row>
     <row r="88" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
@@ -3578,7 +3586,7 @@
       <c r="D88" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E88" s="6" t="s">
+      <c r="E88" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -3595,7 +3603,7 @@
       <c r="D89" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E89" s="6"/>
+      <c r="E89" s="4"/>
     </row>
     <row r="90" spans="1:6" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
@@ -3610,7 +3618,7 @@
       <c r="D90" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E90" s="6" t="s">
+      <c r="E90" s="4" t="s">
         <v>411</v>
       </c>
     </row>
@@ -3627,7 +3635,7 @@
       <c r="D91" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E91" s="6"/>
+      <c r="E91" s="4"/>
     </row>
     <row r="92" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
@@ -3642,7 +3650,7 @@
       <c r="D92" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E92" s="6"/>
+      <c r="E92" s="4"/>
     </row>
     <row r="93" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
@@ -3657,7 +3665,7 @@
       <c r="D93" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E93" s="6"/>
+      <c r="E93" s="4"/>
     </row>
     <row r="94" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
@@ -3672,11 +3680,11 @@
       <c r="D94" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E94" s="6" t="s">
-        <v>441</v>
+      <c r="E94" s="4" t="s">
+        <v>445</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="95" spans="1:6" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3692,7 +3700,7 @@
       <c r="D95" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E95" s="6"/>
+      <c r="E95" s="4"/>
     </row>
     <row r="96" spans="1:6" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
@@ -3707,7 +3715,7 @@
       <c r="D96" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E96" s="6"/>
+      <c r="E96" s="4"/>
     </row>
     <row r="97" spans="1:5" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
@@ -3722,7 +3730,7 @@
       <c r="D97" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E97" s="6"/>
+      <c r="E97" s="4"/>
     </row>
     <row r="98" spans="1:5" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
@@ -3737,7 +3745,7 @@
       <c r="D98" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E98" s="6"/>
+      <c r="E98" s="4"/>
     </row>
     <row r="99" spans="1:5" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
@@ -3752,7 +3760,7 @@
       <c r="D99" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E99" s="6" t="s">
+      <c r="E99" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -3769,7 +3777,7 @@
       <c r="D100" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E100" s="6"/>
+      <c r="E100" s="4"/>
     </row>
     <row r="101" spans="1:5" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
@@ -3784,7 +3792,7 @@
       <c r="D101" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E101" s="6"/>
+      <c r="E101" s="4"/>
     </row>
     <row r="102" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
@@ -3799,7 +3807,7 @@
       <c r="D102" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E102" s="6"/>
+      <c r="E102" s="4"/>
     </row>
     <row r="103" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
@@ -3814,7 +3822,7 @@
       <c r="D103" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E103" s="6" t="s">
+      <c r="E103" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -3831,7 +3839,7 @@
       <c r="D104" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E104" s="6" t="s">
+      <c r="E104" s="4" t="s">
         <v>415</v>
       </c>
     </row>
@@ -3848,7 +3856,7 @@
       <c r="D105" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E105" s="6"/>
+      <c r="E105" s="4"/>
     </row>
     <row r="106" spans="1:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
@@ -3863,7 +3871,7 @@
       <c r="D106" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E106" s="6"/>
+      <c r="E106" s="4"/>
     </row>
     <row r="107" spans="1:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
@@ -3878,7 +3886,7 @@
       <c r="D107" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E107" s="6"/>
+      <c r="E107" s="4"/>
     </row>
     <row r="108" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
@@ -3893,7 +3901,7 @@
       <c r="D108" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E108" s="6" t="s">
+      <c r="E108" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -3910,7 +3918,7 @@
       <c r="D109" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E109" s="6"/>
+      <c r="E109" s="4"/>
     </row>
     <row r="110" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
@@ -3925,7 +3933,7 @@
       <c r="D110" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E110" s="6"/>
+      <c r="E110" s="4"/>
     </row>
     <row r="111" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
@@ -3940,7 +3948,7 @@
       <c r="D111" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E111" s="6" t="s">
+      <c r="E111" s="4" t="s">
         <v>416</v>
       </c>
     </row>
@@ -3957,7 +3965,7 @@
       <c r="D112" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="E112" s="6"/>
+      <c r="E112" s="4"/>
     </row>
     <row r="113" spans="1:5" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
@@ -3972,7 +3980,7 @@
       <c r="D113" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E113" s="6" t="s">
+      <c r="E113" s="4" t="s">
         <v>417</v>
       </c>
     </row>
@@ -3989,7 +3997,7 @@
       <c r="D114" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E114" s="6" t="s">
+      <c r="E114" s="4" t="s">
         <v>418</v>
       </c>
     </row>
@@ -4006,7 +4014,7 @@
       <c r="D115" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E115" s="6"/>
+      <c r="E115" s="4"/>
     </row>
     <row r="116" spans="1:5" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
@@ -4021,7 +4029,7 @@
       <c r="D116" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E116" s="6" t="s">
+      <c r="E116" s="4" t="s">
         <v>419</v>
       </c>
     </row>
@@ -4038,7 +4046,7 @@
       <c r="D117" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E117" s="6" t="s">
+      <c r="E117" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -4055,7 +4063,7 @@
       <c r="D118" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E118" s="6"/>
+      <c r="E118" s="4"/>
     </row>
     <row r="119" spans="1:5" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
@@ -4070,7 +4078,7 @@
       <c r="D119" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E119" s="6"/>
+      <c r="E119" s="4"/>
     </row>
     <row r="120" spans="1:5" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
@@ -4085,7 +4093,7 @@
       <c r="D120" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E120" s="6" t="s">
+      <c r="E120" s="4" t="s">
         <v>420</v>
       </c>
     </row>
@@ -4102,7 +4110,7 @@
       <c r="D121" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E121" s="6"/>
+      <c r="E121" s="4"/>
     </row>
     <row r="122" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
@@ -4117,7 +4125,7 @@
       <c r="D122" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E122" s="6"/>
+      <c r="E122" s="4"/>
     </row>
     <row r="123" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
@@ -4132,7 +4140,7 @@
       <c r="D123" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E123" s="6"/>
+      <c r="E123" s="4"/>
     </row>
     <row r="124" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
@@ -4147,7 +4155,7 @@
       <c r="D124" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E124" s="6"/>
+      <c r="E124" s="4"/>
     </row>
     <row r="125" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
@@ -4162,7 +4170,7 @@
       <c r="D125" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E125" s="6"/>
+      <c r="E125" s="4"/>
     </row>
     <row r="126" spans="1:5" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
@@ -4177,7 +4185,7 @@
       <c r="D126" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E126" s="6"/>
+      <c r="E126" s="4"/>
     </row>
     <row r="127" spans="1:5" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
@@ -4192,7 +4200,7 @@
       <c r="D127" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E127" s="6"/>
+      <c r="E127" s="4"/>
     </row>
     <row r="128" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
@@ -4207,7 +4215,7 @@
       <c r="D128" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E128" s="6"/>
+      <c r="E128" s="4"/>
     </row>
     <row r="129" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
@@ -4222,7 +4230,7 @@
       <c r="D129" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E129" s="6"/>
+      <c r="E129" s="4"/>
     </row>
     <row r="130" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
@@ -4237,7 +4245,7 @@
       <c r="D130" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E130" s="6" t="s">
+      <c r="E130" s="4" t="s">
         <v>422</v>
       </c>
     </row>
@@ -4254,7 +4262,7 @@
       <c r="D131" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E131" s="6" t="s">
+      <c r="E131" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -4271,7 +4279,7 @@
       <c r="D132" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E132" s="6" t="s">
+      <c r="E132" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -4288,7 +4296,7 @@
       <c r="D133" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E133" s="6" t="s">
+      <c r="E133" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -4305,7 +4313,7 @@
       <c r="D134" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E134" s="6" t="s">
+      <c r="E134" s="4" t="s">
         <v>421</v>
       </c>
     </row>
@@ -4322,7 +4330,7 @@
       <c r="D135" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E135" s="6" t="s">
+      <c r="E135" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -4339,7 +4347,7 @@
       <c r="D136" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="E136" s="6"/>
+      <c r="E136" s="4"/>
     </row>
   </sheetData>
   <sortState ref="A2:E136">

</xml_diff>